<commit_message>
- Test with Matlab showed same results, given Matlab not loading the FITS files properly. -  Fixed qualitative colormap for the ball-based color labeling.
</commit_message>
<xml_diff>
--- a/excel_sheets/ball_force_test.xlsx
+++ b/excel_sheets/ball_force_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rattie/Dev/sdo_tracking_framework/excel_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C775B645-F313-C84C-9978-DFEE9B08C8E8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A8B421-D4AC-CC4E-85C1-1E2A11DCDF3C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17260" yWindow="2580" windowWidth="17780" windowHeight="17440" xr2:uid="{A3727C7D-4A41-7A40-B3E9-7A95AD64C0BC}"/>
+    <workbookView xWindow="420" yWindow="700" windowWidth="17680" windowHeight="20740" xr2:uid="{A3727C7D-4A41-7A40-B3E9-7A95AD64C0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>height</t>
   </si>
@@ -38,11 +38,26 @@
   <si>
     <t>rows</t>
   </si>
+  <si>
+    <t>k_force</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>(x,y,z)</t>
+  </si>
+  <si>
+    <t>rs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -72,8 +87,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,46 +408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726DBB8C-117F-354B-905A-5E90ABCB5165}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="156" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>-3</v>
-      </c>
-      <c r="B2">
-        <v>-2</v>
-      </c>
-      <c r="C2">
-        <v>-1</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>-3</v>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>-2</v>
       </c>
@@ -443,14 +437,8 @@
       <c r="F3">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>-3</v>
-      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>-2</v>
       </c>
@@ -466,14 +454,8 @@
       <c r="F4">
         <v>2</v>
       </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>-3</v>
-      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>-2</v>
       </c>
@@ -489,14 +471,8 @@
       <c r="F5">
         <v>2</v>
       </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>-3</v>
-      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>-2</v>
       </c>
@@ -512,14 +488,8 @@
       <c r="F6">
         <v>2</v>
       </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>-3</v>
-      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>-2</v>
       </c>
@@ -535,264 +505,527 @@
       <c r="F7">
         <v>2</v>
       </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>-3</v>
-      </c>
-      <c r="B8">
-        <v>-2</v>
-      </c>
-      <c r="C8">
-        <v>-1</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3</v>
-      </c>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
         <v>1</v>
       </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
         <v>0</v>
       </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B13">
+        <v>-1</v>
+      </c>
+      <c r="C13">
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <v>-1</v>
+      </c>
+      <c r="E13">
+        <v>-1</v>
+      </c>
+      <c r="F13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>-2</v>
+      </c>
+      <c r="C14">
+        <v>-2</v>
+      </c>
+      <c r="D14">
+        <v>-2</v>
+      </c>
+      <c r="E14">
+        <v>-2</v>
+      </c>
+      <c r="F14">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>-1</v>
-      </c>
-      <c r="B14">
-        <v>-1</v>
-      </c>
-      <c r="C14">
-        <v>-1</v>
-      </c>
-      <c r="D14">
-        <v>-1</v>
-      </c>
-      <c r="E14">
-        <v>-1</v>
-      </c>
-      <c r="F14">
-        <v>-1</v>
-      </c>
-      <c r="G14">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>-2</v>
-      </c>
-      <c r="B15">
-        <v>-2</v>
-      </c>
-      <c r="C15">
-        <v>-2</v>
-      </c>
-      <c r="D15">
-        <v>-2</v>
-      </c>
-      <c r="E15">
-        <v>-2</v>
-      </c>
-      <c r="F15">
-        <v>-2</v>
-      </c>
-      <c r="G15">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>-3</v>
-      </c>
-      <c r="B16">
-        <v>-3</v>
-      </c>
-      <c r="C16">
-        <v>-3</v>
-      </c>
-      <c r="D16">
-        <v>-3</v>
-      </c>
-      <c r="E16">
-        <v>-3</v>
-      </c>
-      <c r="F16">
-        <v>-3</v>
-      </c>
-      <c r="G16">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>-6.37</v>
-      </c>
-      <c r="B21">
-        <v>-7.11</v>
-      </c>
-      <c r="C21">
-        <v>-7.24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>-9.35</v>
-      </c>
-      <c r="B22">
-        <v>-11.3</v>
-      </c>
-      <c r="C22">
-        <v>-11.3</v>
-      </c>
-      <c r="D22">
+      <c r="B17" s="2">
+        <v>-6.3740863799999996</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-7.10808325</v>
+      </c>
+      <c r="D17" s="2">
+        <v>-7.2427849799999997</v>
+      </c>
+      <c r="E17" s="2">
+        <v>-6.05</v>
+      </c>
+      <c r="F17" s="2">
+        <v>-3.0129418399999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="2">
+        <v>-9.3533430099999997</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-11.346116070000001</v>
+      </c>
+      <c r="D18" s="2">
+        <v>-11.25785065</v>
+      </c>
+      <c r="E18" s="2">
         <v>-8.66</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>-9.65</v>
-      </c>
-      <c r="B23">
-        <v>-13.2</v>
-      </c>
-      <c r="C23">
-        <v>-13.9</v>
-      </c>
-      <c r="D23">
+      <c r="F18" s="2">
+        <v>-4.1184496900000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="2">
+        <v>-9.6535291700000005</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-13.16189</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-13.862</v>
+      </c>
+      <c r="E19" s="2">
         <v>-10.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
+        <v>-6.13209391</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="2">
+        <v>-8.0091323899999995</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-11.99291706</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-12.090300559999999</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-8.6999999999999993</v>
+      </c>
+      <c r="F20" s="2">
+        <v>-4.9035272599999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="2">
+        <v>-5.7512655300000004</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-8.5557584799999997</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-7.8228459399999997</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-5.0290207899999997</v>
+      </c>
+      <c r="F21" s="2">
+        <v>-2.8906695999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="C23" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="D23" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="E23" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="F23" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>-8.01</v>
-      </c>
-      <c r="B24">
-        <v>-12</v>
-      </c>
-      <c r="C24">
-        <v>-12.1</v>
-      </c>
-      <c r="D24">
-        <v>-8.6999999999999993</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C25">
-        <v>-7.82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+        <v>285</v>
+      </c>
+      <c r="B24" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="C24" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="D24" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="E24" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="F24" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>211</v>
+      </c>
+      <c r="B25" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="C25" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="D25" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="E25" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="F25" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="B26" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="C26" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="D26" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="E26" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="F26" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="C27" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="D27" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="E27" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+      <c r="F27" s="3">
+        <v>-12.162232400000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="3">
+        <f>SQRT(B3^2+B10^2 + (B23-B17)^2)</f>
+        <v>6.4422538252417416</v>
+      </c>
+      <c r="C32" s="3">
+        <f t="shared" ref="C32:F32" si="0">SQRT(C3^2+C10^2 + (C23-C17)^2)</f>
+        <v>5.5267009716869726</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>5.3104578821552355</v>
+      </c>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>6.5084087849189203</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="0"/>
+        <v>9.5765086410082212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="3">
+        <f t="shared" ref="B33:F33" si="1">SQRT(B4^2+B11^2 + (B24-B18)^2)</f>
+        <v>3.5902450620054585</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" si="1"/>
+        <v>1.6328030695992302</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="1"/>
+        <v>1.3482975746225547</v>
+      </c>
+      <c r="E33" s="3">
+        <f t="shared" si="1"/>
+        <v>3.7769871304532878</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="1"/>
+        <v>8.3487987330929805</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="3">
+        <f t="shared" ref="B34:F34" si="2">SQRT(B5^2+B12^2 + (B25-B19)^2)</f>
+        <v>3.2083628062007628</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="2"/>
+        <v>1.4139714697396684</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="2"/>
+        <v>1.6997675999999995</v>
+      </c>
+      <c r="E34" s="3">
+        <f t="shared" si="2"/>
+        <v>1.7714749762866435</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>6.3531543510747071</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="3">
+        <f t="shared" ref="B35:F35" si="3">SQRT(B6^2+B13^2 + (B26-B20)^2)</f>
+        <v>4.7168039701753566</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4243130570065403</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0025837569030258</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="3"/>
+        <v>3.7399268965595795</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="3"/>
+        <v>7.5953143654138788</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="3">
+        <f t="shared" ref="B36:F36" si="4">SQRT(B7^2+B14^2 + (B27-B21)^2)</f>
+        <v>7.0071746237865087</v>
+      </c>
+      <c r="C36" s="3">
+        <f t="shared" si="4"/>
+        <v>4.2434248120639735</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="4"/>
+        <v>4.7781036875764151</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="4"/>
+        <v>7.4754737557588147</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="4"/>
+        <v>9.6933934591733077</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="3">
+        <f>B32-$A$39</f>
+        <v>4.4422538252417416</v>
+      </c>
+      <c r="C40" s="3">
+        <f t="shared" ref="C40:F40" si="5">C32-$A$39</f>
+        <v>3.5267009716869726</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="5"/>
+        <v>3.3104578821552355</v>
+      </c>
+      <c r="E40" s="3">
+        <f t="shared" si="5"/>
+        <v>4.5084087849189203</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="5"/>
+        <v>7.5765086410082212</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="3">
+        <f t="shared" ref="B41:F41" si="6">B33-$A$39</f>
+        <v>1.5902450620054585</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="shared" si="6"/>
+        <v>-0.36719693040076984</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="6"/>
+        <v>-0.65170242537744527</v>
+      </c>
+      <c r="E41" s="3">
+        <f t="shared" si="6"/>
+        <v>1.7769871304532878</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="6"/>
+        <v>6.3487987330929805</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="3">
+        <f t="shared" ref="B42:F42" si="7">B34-$A$39</f>
+        <v>1.2083628062007628</v>
+      </c>
+      <c r="C42" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.58602853026033164</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.30023240000000051</v>
+      </c>
+      <c r="E42" s="3">
+        <f t="shared" si="7"/>
+        <v>-0.22852502371335648</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="7"/>
+        <v>4.3531543510747071</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="3">
+        <f t="shared" ref="B43:F44" si="8">B35-$A$39</f>
+        <v>2.7168039701753566</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.57568694299345968</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="8"/>
+        <v>-0.99741624309697419</v>
+      </c>
+      <c r="E43" s="3">
+        <f t="shared" si="8"/>
+        <v>1.7399268965595795</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="8"/>
+        <v>5.5953143654138788</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="3">
+        <f t="shared" si="8"/>
+        <v>5.0071746237865087</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="shared" si="8"/>
+        <v>2.2434248120639735</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="8"/>
+        <v>2.7781036875764151</v>
+      </c>
+      <c r="E44" s="3">
+        <f t="shared" si="8"/>
+        <v>5.4754737557588147</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="8"/>
+        <v>7.6933934591733077</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>0.44209700000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>